<commit_message>
added house cards text file with details of all house cards, house cards class and added note to excel sheet Signed-off-by: bridroberts <brid.roberts@ucdconnect.ie>
</commit_message>
<xml_diff>
--- a/notes/Life Details.xlsx
+++ b/notes/Life Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/brid_roberts_ucdconnect_ie/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B Roberts\OneDrive - University College Dublin\5th Year\SoftwareEngineering\GameOfLife\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34AC3CAE-5BD8-4125-96F8-6EB827EE9EE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD205AC-1B90-4340-A802-D652625D1A2E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{0D800C94-CC31-4507-93F3-CCA87D1A34F0}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>User Stories</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>RETIREMENT: order of retirement; loan repayment; sell houses; collect money for action cards; collect money for children; winner = wealthiest</t>
+  </si>
+  <si>
+    <t>functions: remove a house, read in houses, get house details</t>
   </si>
 </sst>
 </file>
@@ -600,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD92DF88-46EF-4350-B7DB-4332BB3D015A}">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,6 +612,7 @@
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" customWidth="1"/>
     <col min="3" max="3" width="61.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -740,12 +744,15 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Created InitialiseGame class in order to initialise card decks and players cleanly (outside of main!) - Updated player, card and spinner classes in order to accomodate the InitialiseGame class - Created Utility, Space and BoardReader in order to read in spaces which will make up teh board - Implemented the first part of 'moving' a player in main Signed-off-by: bridroberts <brid.roberts@ucdconnect.ie>
</commit_message>
<xml_diff>
--- a/notes/Life Details.xlsx
+++ b/notes/Life Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B Roberts\OneDrive - University College Dublin\5th Year\SoftwareEngineering\GameOfLife\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD205AC-1B90-4340-A802-D652625D1A2E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C5FB22-C827-4C14-B249-7C568985F467}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{0D800C94-CC31-4507-93F3-CCA87D1A34F0}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>User Stories</t>
   </si>
@@ -210,6 +210,24 @@
   </si>
   <si>
     <t>functions: remove a house, read in houses, get house details</t>
+  </si>
+  <si>
+    <t>STEPS:</t>
+  </si>
+  <si>
+    <t>2) Spin Spinner</t>
+  </si>
+  <si>
+    <t>3) Move specified number of spaces</t>
+  </si>
+  <si>
+    <t>1) Initialise Players,</t>
+  </si>
+  <si>
+    <t>4) Complete action indicated by space</t>
+  </si>
+  <si>
+    <t>5) Next player</t>
   </si>
 </sst>
 </file>
@@ -275,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -286,6 +304,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -601,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD92DF88-46EF-4350-B7DB-4332BB3D015A}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,6 +960,40 @@
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="6"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="6"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" s="6"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="6"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="F1:H6"/>

</xml_diff>